<commit_message>
all temperature measurements in excel files
</commit_message>
<xml_diff>
--- a/pile5_sect_1_all.xlsx
+++ b/pile5_sect_1_all.xlsx
@@ -524,7 +524,7 @@
         <v>44065</v>
       </c>
       <c r="B6">
-        <v>31.91583333333333</v>
+        <v>31.91583333333334</v>
       </c>
       <c r="C6">
         <v>33.74083333333333</v>
@@ -579,7 +579,7 @@
         <v>29.8925</v>
       </c>
       <c r="E8">
-        <v>15.49416666666666</v>
+        <v>15.49416666666667</v>
       </c>
       <c r="F8">
         <v>81.625</v>
@@ -593,7 +593,7 @@
         <v>44068</v>
       </c>
       <c r="B9">
-        <v>28.81083333333334</v>
+        <v>28.81083333333333</v>
       </c>
       <c r="C9">
         <v>30.45833333333333</v>
@@ -622,7 +622,7 @@
         <v>29.16208333333333</v>
       </c>
       <c r="D10">
-        <v>31.16166666666666</v>
+        <v>31.16166666666667</v>
       </c>
       <c r="E10">
         <v>13.62833333333333</v>
@@ -639,7 +639,7 @@
         <v>44070</v>
       </c>
       <c r="B11">
-        <v>26.39958333333333</v>
+        <v>26.39958333333334</v>
       </c>
       <c r="C11">
         <v>27.81791666666667</v>
@@ -665,7 +665,7 @@
         <v>26.10333333333334</v>
       </c>
       <c r="C12">
-        <v>27.48333333333334</v>
+        <v>27.48333333333333</v>
       </c>
       <c r="D12">
         <v>28.14416666666667</v>
@@ -688,13 +688,13 @@
         <v>25.72875</v>
       </c>
       <c r="C13">
-        <v>27.29500000000001</v>
+        <v>27.295</v>
       </c>
       <c r="D13">
-        <v>27.79708333333334</v>
+        <v>27.79708333333333</v>
       </c>
       <c r="E13">
-        <v>13.90666666666666</v>
+        <v>13.90666666666667</v>
       </c>
       <c r="F13">
         <v>77</v>
@@ -708,13 +708,13 @@
         <v>44073</v>
       </c>
       <c r="B14">
-        <v>25.89666666666667</v>
+        <v>25.89666666666666</v>
       </c>
       <c r="C14">
         <v>27.14291666666666</v>
       </c>
       <c r="D14">
-        <v>27.19874999999999</v>
+        <v>27.19875</v>
       </c>
       <c r="E14">
         <v>14.00916666666667</v>
@@ -731,16 +731,16 @@
         <v>44074</v>
       </c>
       <c r="B15">
-        <v>26.87124999999999</v>
+        <v>26.87125</v>
       </c>
       <c r="C15">
-        <v>28.16416666666666</v>
+        <v>28.16416666666667</v>
       </c>
       <c r="D15">
-        <v>25.23958333333334</v>
+        <v>25.23958333333333</v>
       </c>
       <c r="E15">
-        <v>14.04916666666666</v>
+        <v>14.04916666666667</v>
       </c>
       <c r="F15">
         <v>73.5</v>
@@ -754,10 +754,10 @@
         <v>44075</v>
       </c>
       <c r="B16">
-        <v>26.59291666666666</v>
+        <v>26.59291666666667</v>
       </c>
       <c r="C16">
-        <v>28.26583333333334</v>
+        <v>28.26583333333333</v>
       </c>
       <c r="D16">
         <v>24.22791666666667</v>
@@ -780,7 +780,7 @@
         <v>26.46458333333333</v>
       </c>
       <c r="C17">
-        <v>27.80249999999999</v>
+        <v>27.8025</v>
       </c>
       <c r="D17">
         <v>24.77583333333333</v>
@@ -829,7 +829,7 @@
         <v>26.22208333333333</v>
       </c>
       <c r="D19">
-        <v>22.71583333333334</v>
+        <v>22.71583333333333</v>
       </c>
       <c r="E19">
         <v>16.56791666666667</v>
@@ -846,7 +846,7 @@
         <v>44079</v>
       </c>
       <c r="B20">
-        <v>25.66458333333333</v>
+        <v>25.66458333333334</v>
       </c>
       <c r="C20">
         <v>26.50625</v>
@@ -861,7 +861,7 @@
         <v>85.41666666666667</v>
       </c>
       <c r="G20">
-        <v>4.400000000000001</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -869,10 +869,10 @@
         <v>44080</v>
       </c>
       <c r="B21">
-        <v>26.09791666666666</v>
+        <v>26.09791666666667</v>
       </c>
       <c r="C21">
-        <v>26.92374999999999</v>
+        <v>26.92375</v>
       </c>
       <c r="D21">
         <v>22.12041666666667</v>
@@ -892,13 +892,13 @@
         <v>44081</v>
       </c>
       <c r="B22">
-        <v>26.06833333333334</v>
+        <v>26.06833333333333</v>
       </c>
       <c r="C22">
         <v>27.04916666666666</v>
       </c>
       <c r="D22">
-        <v>23.40083333333334</v>
+        <v>23.40083333333333</v>
       </c>
       <c r="E22">
         <v>13.09291666666667</v>
@@ -918,10 +918,10 @@
         <v>25.87833333333333</v>
       </c>
       <c r="C23">
-        <v>26.80250000000001</v>
+        <v>26.8025</v>
       </c>
       <c r="D23">
-        <v>24.19333333333334</v>
+        <v>24.19333333333333</v>
       </c>
       <c r="E23">
         <v>11.05941666666667</v>
@@ -941,7 +941,7 @@
         <v>25.24791666666667</v>
       </c>
       <c r="C24">
-        <v>26.22666666666666</v>
+        <v>26.22666666666667</v>
       </c>
       <c r="D24">
         <v>24.835</v>
@@ -987,13 +987,13 @@
         <v>24.28</v>
       </c>
       <c r="C26">
-        <v>25.55958333333334</v>
+        <v>25.55958333333333</v>
       </c>
       <c r="D26">
         <v>22.11416666666667</v>
       </c>
       <c r="E26">
-        <v>9.641958333333331</v>
+        <v>9.641958333333333</v>
       </c>
       <c r="F26">
         <v>83.04166666666667</v>
@@ -1030,7 +1030,7 @@
         <v>44087</v>
       </c>
       <c r="B28">
-        <v>21.97291666666666</v>
+        <v>21.97291666666667</v>
       </c>
       <c r="C28">
         <v>21.72083333333333</v>
@@ -1045,7 +1045,7 @@
         <v>82.33333333333333</v>
       </c>
       <c r="G28">
-        <v>9.799999999999999</v>
+        <v>9.800000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1056,10 +1056,10 @@
         <v>19.73458333333333</v>
       </c>
       <c r="C29">
-        <v>18.04208333333334</v>
+        <v>18.04208333333333</v>
       </c>
       <c r="D29">
-        <v>25.68708333333334</v>
+        <v>25.68708333333333</v>
       </c>
       <c r="E29">
         <v>11.25125</v>
@@ -1079,10 +1079,10 @@
         <v>19.61125</v>
       </c>
       <c r="C30">
-        <v>17.97958333333334</v>
+        <v>17.97958333333333</v>
       </c>
       <c r="D30">
-        <v>25.38458333333333</v>
+        <v>25.38458333333334</v>
       </c>
       <c r="E30">
         <v>10.424</v>
@@ -1099,16 +1099,16 @@
         <v>44090</v>
       </c>
       <c r="B31">
-        <v>21.99291666666666</v>
+        <v>21.99291666666667</v>
       </c>
       <c r="C31">
         <v>21.07916666666667</v>
       </c>
       <c r="D31">
-        <v>22.26375000000001</v>
+        <v>22.26375</v>
       </c>
       <c r="E31">
-        <v>9.808458333333334</v>
+        <v>9.808458333333332</v>
       </c>
       <c r="F31">
         <v>93.45833333333333</v>
@@ -1125,7 +1125,7 @@
         <v>23.61875</v>
       </c>
       <c r="C32">
-        <v>23.28374999999999</v>
+        <v>23.28375</v>
       </c>
       <c r="D32">
         <v>14.01875</v>
@@ -1154,7 +1154,7 @@
         <v>11.21125</v>
       </c>
       <c r="E33">
-        <v>8.436250000000001</v>
+        <v>8.436249999999999</v>
       </c>
       <c r="F33">
         <v>79.875</v>
@@ -1168,7 +1168,7 @@
         <v>44093</v>
       </c>
       <c r="B34">
-        <v>23.17791666666667</v>
+        <v>23.17791666666666</v>
       </c>
       <c r="C34">
         <v>23.3675</v>
@@ -1194,13 +1194,13 @@
         <v>21.32458333333333</v>
       </c>
       <c r="C35">
-        <v>20.29124999999999</v>
+        <v>20.29125</v>
       </c>
       <c r="D35">
         <v>15.91</v>
       </c>
       <c r="E35">
-        <v>8.898416666666664</v>
+        <v>8.898416666666668</v>
       </c>
       <c r="F35">
         <v>78.875</v>
@@ -1217,7 +1217,7 @@
         <v>19.58458333333333</v>
       </c>
       <c r="C36">
-        <v>16.86833333333334</v>
+        <v>16.86833333333333</v>
       </c>
       <c r="D36">
         <v>19.355</v>
@@ -1246,7 +1246,7 @@
         <v>22.44541666666666</v>
       </c>
       <c r="E37">
-        <v>10.81533333333334</v>
+        <v>10.81533333333333</v>
       </c>
       <c r="F37">
         <v>70.125</v>
@@ -1286,13 +1286,13 @@
         <v>19.9475</v>
       </c>
       <c r="C39">
-        <v>17.90333333333334</v>
+        <v>17.90333333333333</v>
       </c>
       <c r="D39">
         <v>20.10416666666667</v>
       </c>
       <c r="E39">
-        <v>12.02708333333334</v>
+        <v>12.02708333333333</v>
       </c>
       <c r="F39">
         <v>94.66666666666667</v>
@@ -1375,7 +1375,7 @@
         <v>44102</v>
       </c>
       <c r="B43">
-        <v>23.08541666666667</v>
+        <v>23.08541666666666</v>
       </c>
       <c r="C43">
         <v>23.05708333333333</v>
@@ -1398,7 +1398,7 @@
         <v>44103</v>
       </c>
       <c r="B44">
-        <v>22.84000000000001</v>
+        <v>22.84</v>
       </c>
       <c r="C44">
         <v>23.27791666666667</v>
@@ -1430,7 +1430,7 @@
         <v>23.53958333333334</v>
       </c>
       <c r="E45">
-        <v>11.40041666666666</v>
+        <v>11.40041666666667</v>
       </c>
       <c r="F45">
         <v>91.41666666666667</v>
@@ -1467,16 +1467,16 @@
         <v>44106</v>
       </c>
       <c r="B47">
-        <v>23.10208333333333</v>
+        <v>23.10208333333334</v>
       </c>
       <c r="C47">
         <v>24.23125</v>
       </c>
       <c r="D47">
-        <v>24.07541666666666</v>
+        <v>24.07541666666667</v>
       </c>
       <c r="E47">
-        <v>10.73166666666666</v>
+        <v>10.73166666666667</v>
       </c>
       <c r="F47">
         <v>88.33333333333333</v>
@@ -1493,7 +1493,7 @@
         <v>22.79</v>
       </c>
       <c r="C48">
-        <v>24.08458333333334</v>
+        <v>24.08458333333333</v>
       </c>
       <c r="D48">
         <v>23.8575</v>
@@ -1591,7 +1591,7 @@
         <v>18.15583333333333</v>
       </c>
       <c r="E52">
-        <v>11.91708333333334</v>
+        <v>11.91708333333333</v>
       </c>
       <c r="F52">
         <v>90.29166666666667</v>
@@ -1611,7 +1611,7 @@
         <v>17.90791666666667</v>
       </c>
       <c r="D53">
-        <v>18.21250000000001</v>
+        <v>18.2125</v>
       </c>
       <c r="E53">
         <v>11.76916666666667</v>
@@ -1628,7 +1628,7 @@
         <v>44113</v>
       </c>
       <c r="B54">
-        <v>17.57958333333333</v>
+        <v>17.57958333333334</v>
       </c>
       <c r="C54">
         <v>18.86041666666667</v>
@@ -1660,7 +1660,7 @@
         <v>19.33333333333333</v>
       </c>
       <c r="E55">
-        <v>9.957500000000001</v>
+        <v>9.9575</v>
       </c>
       <c r="F55">
         <v>82.29166666666667</v>
@@ -1680,16 +1680,16 @@
         <v>21.08208333333333</v>
       </c>
       <c r="D56">
-        <v>20.73666666666666</v>
+        <v>20.73666666666667</v>
       </c>
       <c r="E56">
-        <v>8.823416666666665</v>
+        <v>8.823416666666667</v>
       </c>
       <c r="F56">
         <v>93.79166666666667</v>
       </c>
       <c r="G56">
-        <v>5.800000000000001</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1703,10 +1703,10 @@
         <v>21.32125</v>
       </c>
       <c r="D57">
-        <v>22.05333333333334</v>
+        <v>22.05333333333333</v>
       </c>
       <c r="E57">
-        <v>8.284124999999998</v>
+        <v>8.284125</v>
       </c>
       <c r="F57">
         <v>95.08333333333333</v>
@@ -1726,7 +1726,7 @@
         <v>21.32583333333333</v>
       </c>
       <c r="D58">
-        <v>23.05958333333334</v>
+        <v>23.05958333333333</v>
       </c>
       <c r="E58">
         <v>8.141958333333333</v>
@@ -1746,13 +1746,13 @@
         <v>20.14708333333333</v>
       </c>
       <c r="C59">
-        <v>21.32083333333334</v>
+        <v>21.32083333333333</v>
       </c>
       <c r="D59">
         <v>21.52083333333333</v>
       </c>
       <c r="E59">
-        <v>5.322166666666666</v>
+        <v>5.322166666666667</v>
       </c>
       <c r="F59">
         <v>87.375</v>
@@ -1812,7 +1812,7 @@
         <v>44121</v>
       </c>
       <c r="B62">
-        <v>16.14291666666666</v>
+        <v>16.14291666666667</v>
       </c>
       <c r="C62">
         <v>15.16708333333333</v>
@@ -1821,7 +1821,7 @@
         <v>20.85291666666667</v>
       </c>
       <c r="E62">
-        <v>4.374166666666666</v>
+        <v>4.374166666666667</v>
       </c>
       <c r="F62">
         <v>91.95833333333333</v>
@@ -1881,7 +1881,7 @@
         <v>44124</v>
       </c>
       <c r="B65">
-        <v>15.09791666666666</v>
+        <v>15.09791666666667</v>
       </c>
       <c r="C65">
         <v>15.7525</v>
@@ -1890,7 +1890,7 @@
         <v>12.61041666666667</v>
       </c>
       <c r="E65">
-        <v>0.1062916666666666</v>
+        <v>0.1062916666666667</v>
       </c>
       <c r="F65">
         <v>85.5</v>
@@ -1904,7 +1904,7 @@
         <v>44125</v>
       </c>
       <c r="B66">
-        <v>15.21541666666666</v>
+        <v>15.21541666666667</v>
       </c>
       <c r="C66">
         <v>14.10333333333333</v>
@@ -1913,13 +1913,13 @@
         <v>14.00666666666667</v>
       </c>
       <c r="E66">
-        <v>0.5442499999999999</v>
+        <v>0.54425</v>
       </c>
       <c r="F66">
         <v>87.125</v>
       </c>
       <c r="G66">
-        <v>5.400000000000001</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -1933,10 +1933,10 @@
         <v>17.48541666666667</v>
       </c>
       <c r="D67">
-        <v>10.44458333333334</v>
+        <v>10.44458333333333</v>
       </c>
       <c r="E67">
-        <v>4.699583333333332</v>
+        <v>4.699583333333334</v>
       </c>
       <c r="F67">
         <v>95.83333333333333</v>
@@ -1950,13 +1950,13 @@
         <v>44127</v>
       </c>
       <c r="B68">
-        <v>17.60333333333333</v>
+        <v>17.60333333333334</v>
       </c>
       <c r="C68">
         <v>17.34208333333333</v>
       </c>
       <c r="D68">
-        <v>9.182500000000001</v>
+        <v>9.182499999999999</v>
       </c>
       <c r="E68">
         <v>3.38025</v>
@@ -1982,7 +1982,7 @@
         <v>12.08791666666667</v>
       </c>
       <c r="E69">
-        <v>1.863583333333334</v>
+        <v>1.863583333333333</v>
       </c>
       <c r="F69">
         <v>83.20833333333333</v>
@@ -2002,7 +2002,7 @@
         <v>11.79</v>
       </c>
       <c r="D70">
-        <v>13.47166666666666</v>
+        <v>13.47166666666667</v>
       </c>
       <c r="E70">
         <v>1.084916666666667</v>
@@ -2022,13 +2022,13 @@
         <v>17.04916666666667</v>
       </c>
       <c r="C71">
-        <v>15.20041666666666</v>
+        <v>15.20041666666667</v>
       </c>
       <c r="D71">
         <v>10.05041666666667</v>
       </c>
       <c r="E71">
-        <v>7.442125000000001</v>
+        <v>7.442125</v>
       </c>
       <c r="F71">
         <v>91.16666666666667</v>
@@ -2048,7 +2048,7 @@
         <v>17.24416666666667</v>
       </c>
       <c r="D72">
-        <v>8.186291666666664</v>
+        <v>8.186291666666667</v>
       </c>
       <c r="E72">
         <v>9.55875</v>
@@ -2088,13 +2088,13 @@
         <v>44133</v>
       </c>
       <c r="B74">
-        <v>17.83708333333333</v>
+        <v>17.83708333333334</v>
       </c>
       <c r="C74">
         <v>17.61208333333333</v>
       </c>
       <c r="D74">
-        <v>9.882916666666668</v>
+        <v>9.882916666666667</v>
       </c>
       <c r="E74">
         <v>8.209291666666667</v>
@@ -2134,7 +2134,7 @@
         <v>44135</v>
       </c>
       <c r="B76">
-        <v>16.13708333333334</v>
+        <v>16.13708333333333</v>
       </c>
       <c r="C76">
         <v>16.1625</v>
@@ -2143,7 +2143,7 @@
         <v>11.79791666666667</v>
       </c>
       <c r="E76">
-        <v>0.06470833333333344</v>
+        <v>0.06470833333333334</v>
       </c>
       <c r="F76">
         <v>91.04166666666667</v>
@@ -2166,7 +2166,7 @@
         <v>10.89041666666667</v>
       </c>
       <c r="E77">
-        <v>5.111250000000001</v>
+        <v>5.11125</v>
       </c>
       <c r="F77">
         <v>88.41666666666667</v>
@@ -2186,10 +2186,10 @@
         <v>17.04125</v>
       </c>
       <c r="D78">
-        <v>9.120416666666667</v>
+        <v>9.120416666666666</v>
       </c>
       <c r="E78">
-        <v>4.344749999999999</v>
+        <v>4.34475</v>
       </c>
       <c r="F78">
         <v>85.30434782608695</v>
@@ -2209,10 +2209,10 @@
         <v>16.20791666666667</v>
       </c>
       <c r="D79">
-        <v>7.851375000000002</v>
+        <v>7.851375</v>
       </c>
       <c r="E79">
-        <v>8.991499999999998</v>
+        <v>8.9915</v>
       </c>
       <c r="F79">
         <v>88.70833333333333</v>
@@ -2229,10 +2229,10 @@
         <v>16.45625</v>
       </c>
       <c r="C80">
-        <v>16.82083333333334</v>
+        <v>16.82083333333333</v>
       </c>
       <c r="D80">
-        <v>9.925833333333332</v>
+        <v>9.925833333333333</v>
       </c>
       <c r="E80">
         <v>5.958291666666667</v>
@@ -2258,7 +2258,7 @@
         <v>12.77083333333333</v>
       </c>
       <c r="E81">
-        <v>5.708000000000001</v>
+        <v>5.707999999999999</v>
       </c>
       <c r="F81">
         <v>75.875</v>
@@ -2304,7 +2304,7 @@
         <v>17.7375</v>
       </c>
       <c r="E83">
-        <v>8.343624999999999</v>
+        <v>8.343625000000001</v>
       </c>
       <c r="F83">
         <v>71.25</v>
@@ -2321,7 +2321,7 @@
         <v>11.225</v>
       </c>
       <c r="C84">
-        <v>9.746958333333332</v>
+        <v>9.746958333333334</v>
       </c>
       <c r="D84">
         <v>18.17666666666667</v>
@@ -2341,10 +2341,10 @@
         <v>44144</v>
       </c>
       <c r="B85">
-        <v>9.988333333333332</v>
+        <v>9.988333333333333</v>
       </c>
       <c r="C85">
-        <v>9.044166666666666</v>
+        <v>9.044166666666667</v>
       </c>
       <c r="D85">
         <v>18.1225</v>
@@ -2373,7 +2373,7 @@
         <v>17.73875</v>
       </c>
       <c r="E86">
-        <v>-0.8717916666666666</v>
+        <v>-0.8717916666666667</v>
       </c>
       <c r="F86">
         <v>85.45833333333333</v>
@@ -2390,10 +2390,10 @@
         <v>10.26291666666667</v>
       </c>
       <c r="C87">
-        <v>8.794166666666666</v>
+        <v>8.794166666666667</v>
       </c>
       <c r="D87">
-        <v>17.05208333333334</v>
+        <v>17.05208333333333</v>
       </c>
       <c r="E87">
         <v>-0.4385416666666666</v>
@@ -2416,7 +2416,7 @@
         <v>8.455</v>
       </c>
       <c r="D88">
-        <v>16.82041666666666</v>
+        <v>16.82041666666667</v>
       </c>
       <c r="E88">
         <v>2.956208333333333</v>
@@ -2436,13 +2436,13 @@
         <v>11.28791666666667</v>
       </c>
       <c r="C89">
-        <v>8.449583333333335</v>
+        <v>8.449583333333333</v>
       </c>
       <c r="D89">
-        <v>16.55833333333334</v>
+        <v>16.55833333333333</v>
       </c>
       <c r="E89">
-        <v>3.387333333333333</v>
+        <v>3.387333333333334</v>
       </c>
       <c r="F89">
         <v>85.83333333333333</v>
@@ -2459,13 +2459,13 @@
         <v>12.8425</v>
       </c>
       <c r="C90">
-        <v>10.58208333333334</v>
+        <v>10.58208333333333</v>
       </c>
       <c r="D90">
-        <v>15.04291666666667</v>
+        <v>15.04291666666666</v>
       </c>
       <c r="E90">
-        <v>2.419041666666666</v>
+        <v>2.419041666666667</v>
       </c>
       <c r="F90">
         <v>86.54166666666667</v>
@@ -2485,10 +2485,10 @@
         <v>12.57708333333333</v>
       </c>
       <c r="D91">
-        <v>13.02916666666666</v>
+        <v>13.02916666666667</v>
       </c>
       <c r="E91">
-        <v>1.449333333333334</v>
+        <v>1.449333333333333</v>
       </c>
       <c r="F91">
         <v>86.04166666666667</v>
@@ -2534,13 +2534,13 @@
         <v>8.961583333333333</v>
       </c>
       <c r="E93">
-        <v>3.076833333333334</v>
+        <v>3.076833333333333</v>
       </c>
       <c r="F93">
         <v>95.08333333333333</v>
       </c>
       <c r="G93">
-        <v>4.800000000000001</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2554,7 +2554,7 @@
         <v>13.14916666666667</v>
       </c>
       <c r="D94">
-        <v>7.872624999999999</v>
+        <v>7.872625</v>
       </c>
       <c r="E94">
         <v>4.938125</v>
@@ -2580,7 +2580,7 @@
         <v>8.78375</v>
       </c>
       <c r="E95">
-        <v>7.258541666666669</v>
+        <v>7.258541666666667</v>
       </c>
       <c r="F95">
         <v>84.95833333333333</v>
@@ -2617,7 +2617,7 @@
         <v>44156</v>
       </c>
       <c r="B97">
-        <v>11.26833333333334</v>
+        <v>11.26833333333333</v>
       </c>
       <c r="C97">
         <v>9.807499999999999</v>
@@ -2632,7 +2632,7 @@
         <v>91.33333333333333</v>
       </c>
       <c r="G97">
-        <v>3.399999999999999</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2649,7 +2649,7 @@
         <v>8.451708333333334</v>
       </c>
       <c r="E98">
-        <v>2.580124999999999</v>
+        <v>2.580125</v>
       </c>
       <c r="F98">
         <v>91.625</v>
@@ -2666,7 +2666,7 @@
         <v>11.32083333333333</v>
       </c>
       <c r="C99">
-        <v>9.37166666666667</v>
+        <v>9.371666666666668</v>
       </c>
       <c r="D99">
         <v>9.184583333333334</v>
@@ -2715,7 +2715,7 @@
         <v>9.498333333333333</v>
       </c>
       <c r="D101">
-        <v>9.504583333333333</v>
+        <v>9.504583333333334</v>
       </c>
       <c r="E101">
         <v>-2.0205</v>
@@ -2735,7 +2735,7 @@
         <v>11.44041666666667</v>
       </c>
       <c r="C102">
-        <v>9.304166666666669</v>
+        <v>9.304166666666667</v>
       </c>
       <c r="D102">
         <v>9.094458333333334</v>
@@ -2747,7 +2747,7 @@
         <v>91.83333333333333</v>
       </c>
       <c r="G102">
-        <v>7.200000000000001</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -2761,7 +2761,7 @@
         <v>10.42125</v>
       </c>
       <c r="D103">
-        <v>7.464375000000001</v>
+        <v>7.464375</v>
       </c>
       <c r="E103">
         <v>0.3242916666666667</v>
@@ -2778,7 +2778,7 @@
         <v>44163</v>
       </c>
       <c r="B104">
-        <v>12.40458333333334</v>
+        <v>12.40458333333333</v>
       </c>
       <c r="C104">
         <v>11.37458333333333</v>
@@ -2807,7 +2807,7 @@
         <v>11.12625</v>
       </c>
       <c r="D105">
-        <v>7.961750000000001</v>
+        <v>7.961749999999999</v>
       </c>
       <c r="E105">
         <v>-0.6397916666666666</v>
@@ -2830,7 +2830,7 @@
         <v>11.13125</v>
       </c>
       <c r="D106">
-        <v>7.969083333333331</v>
+        <v>7.969083333333334</v>
       </c>
       <c r="E106">
         <v>-0.7167916666666666</v>
@@ -2853,7 +2853,7 @@
         <v>11.01625</v>
       </c>
       <c r="D107">
-        <v>7.369499999999998</v>
+        <v>7.369499999999999</v>
       </c>
       <c r="E107">
         <v>0.2954583333333333</v>
@@ -2873,13 +2873,13 @@
         <v>11.2875</v>
       </c>
       <c r="C108">
-        <v>9.668333333333335</v>
+        <v>9.668333333333333</v>
       </c>
       <c r="D108">
-        <v>8.464500000000001</v>
+        <v>8.464499999999999</v>
       </c>
       <c r="E108">
-        <v>0.04624999999999996</v>
+        <v>0.04625000000000001</v>
       </c>
       <c r="F108">
         <v>91</v>
@@ -2899,7 +2899,7 @@
         <v>10.77125</v>
       </c>
       <c r="D109">
-        <v>6.794541666666667</v>
+        <v>6.794541666666666</v>
       </c>
       <c r="E109">
         <v>-1.112708333333333</v>
@@ -2925,7 +2925,7 @@
         <v>6.030041666666667</v>
       </c>
       <c r="E110">
-        <v>-0.8550833333333331</v>
+        <v>-0.8550833333333333</v>
       </c>
       <c r="F110">
         <v>84.875</v>
@@ -2968,10 +2968,10 @@
         <v>11.67416666666667</v>
       </c>
       <c r="D112">
-        <v>4.668291666666666</v>
+        <v>4.668291666666667</v>
       </c>
       <c r="E112">
-        <v>2.182333333333334</v>
+        <v>2.182333333333333</v>
       </c>
       <c r="F112">
         <v>96.70833333333333</v>
@@ -3014,7 +3014,7 @@
         <v>11.15416666666667</v>
       </c>
       <c r="D114">
-        <v>4.671833333333334</v>
+        <v>4.671833333333333</v>
       </c>
       <c r="E114">
         <v>-3.088958333333334</v>
@@ -3034,13 +3034,13 @@
         <v>10.53125</v>
       </c>
       <c r="C115">
-        <v>10.66541666666666</v>
+        <v>10.66541666666667</v>
       </c>
       <c r="D115">
         <v>4.653291666666667</v>
       </c>
       <c r="E115">
-        <v>-3.974291666666668</v>
+        <v>-3.974291666666666</v>
       </c>
       <c r="F115">
         <v>83.125</v>
@@ -3060,10 +3060,10 @@
         <v>10.24708333333333</v>
       </c>
       <c r="D116">
-        <v>4.651166666666668</v>
+        <v>4.651166666666667</v>
       </c>
       <c r="E116">
-        <v>-3.702916666666666</v>
+        <v>-3.702916666666667</v>
       </c>
       <c r="F116">
         <v>86.33333333333333</v>
@@ -3083,10 +3083,10 @@
         <v>9.793750000000001</v>
       </c>
       <c r="D117">
-        <v>5.106000000000001</v>
+        <v>5.106</v>
       </c>
       <c r="E117">
-        <v>-4.134375000000001</v>
+        <v>-4.134374999999999</v>
       </c>
       <c r="F117">
         <v>87.83333333333333</v>
@@ -3100,7 +3100,7 @@
         <v>44177</v>
       </c>
       <c r="B118">
-        <v>9.434166666666664</v>
+        <v>9.434166666666666</v>
       </c>
       <c r="C118">
         <v>9.43</v>
@@ -3132,7 +3132,7 @@
         <v>5.179916666666666</v>
       </c>
       <c r="E119">
-        <v>-2.910874999999999</v>
+        <v>-2.910875</v>
       </c>
       <c r="F119">
         <v>89.75</v>
@@ -3146,7 +3146,7 @@
         <v>44179</v>
       </c>
       <c r="B120">
-        <v>9.233333333333329</v>
+        <v>9.233333333333333</v>
       </c>
       <c r="C120">
         <v>9.117916666666668</v>
@@ -3169,16 +3169,16 @@
         <v>44180</v>
       </c>
       <c r="B121">
-        <v>9.242916666666668</v>
+        <v>9.242916666666666</v>
       </c>
       <c r="C121">
         <v>9.03125</v>
       </c>
       <c r="D121">
-        <v>5.572583333333335</v>
+        <v>5.572583333333333</v>
       </c>
       <c r="E121">
-        <v>-2.689583333333334</v>
+        <v>-2.689583333333333</v>
       </c>
       <c r="F121">
         <v>91.08333333333333</v>
@@ -3192,10 +3192,10 @@
         <v>44181</v>
       </c>
       <c r="B122">
-        <v>9.382916666666665</v>
+        <v>9.382916666666667</v>
       </c>
       <c r="C122">
-        <v>9.249583333333337</v>
+        <v>9.249583333333332</v>
       </c>
       <c r="D122">
         <v>5.082208333333333</v>
@@ -3221,7 +3221,7 @@
         <v>9.337916666666667</v>
       </c>
       <c r="D123">
-        <v>4.872249999999999</v>
+        <v>4.87225</v>
       </c>
       <c r="E123">
         <v>-2.231458333333333</v>
@@ -3241,7 +3241,7 @@
         <v>8.817083333333334</v>
       </c>
       <c r="C124">
-        <v>8.992916666666668</v>
+        <v>8.992916666666666</v>
       </c>
       <c r="D124">
         <v>5.078041666666667</v>
@@ -3261,7 +3261,7 @@
         <v>44184</v>
       </c>
       <c r="B125">
-        <v>8.240416666666668</v>
+        <v>8.240416666666667</v>
       </c>
       <c r="C125">
         <v>8.534166666666666</v>
@@ -3270,7 +3270,7 @@
         <v>4.885625</v>
       </c>
       <c r="E125">
-        <v>-1.485458333333333</v>
+        <v>-1.485458333333334</v>
       </c>
       <c r="F125">
         <v>94.95833333333333</v>
@@ -3284,7 +3284,7 @@
         <v>44185</v>
       </c>
       <c r="B126">
-        <v>8.375833333333331</v>
+        <v>8.375833333333333</v>
       </c>
       <c r="C126">
         <v>8.765416666666667</v>
@@ -3307,7 +3307,7 @@
         <v>44186</v>
       </c>
       <c r="B127">
-        <v>8.722500000000002</v>
+        <v>8.7225</v>
       </c>
       <c r="C127">
         <v>8.990416666666667</v>
@@ -3330,13 +3330,13 @@
         <v>44187</v>
       </c>
       <c r="B128">
-        <v>8.913749999999999</v>
+        <v>8.91375</v>
       </c>
       <c r="C128">
         <v>9.077499999999999</v>
       </c>
       <c r="D128">
-        <v>6.094958333333332</v>
+        <v>6.094958333333333</v>
       </c>
       <c r="E128">
         <v>2.614416666666667</v>
@@ -3353,7 +3353,7 @@
         <v>44188</v>
       </c>
       <c r="B129">
-        <v>8.811250000000001</v>
+        <v>8.811249999999999</v>
       </c>
       <c r="C129">
         <v>9.497083333333334</v>
@@ -3362,7 +3362,7 @@
         <v>5.485875</v>
       </c>
       <c r="E129">
-        <v>-0.02837500000000002</v>
+        <v>-0.02837499999999999</v>
       </c>
       <c r="F129">
         <v>94.75</v>
@@ -3379,13 +3379,13 @@
         <v>8.733333333333333</v>
       </c>
       <c r="C130">
-        <v>9.226249999999999</v>
+        <v>9.22625</v>
       </c>
       <c r="D130">
-        <v>5.283749999999999</v>
+        <v>5.28375</v>
       </c>
       <c r="E130">
-        <v>-0.5793749999999999</v>
+        <v>-0.579375</v>
       </c>
       <c r="F130">
         <v>96.375</v>
@@ -3399,10 +3399,10 @@
         <v>44190</v>
       </c>
       <c r="B131">
-        <v>8.52958333333333</v>
+        <v>8.529583333333333</v>
       </c>
       <c r="C131">
-        <v>8.858749999999999</v>
+        <v>8.858750000000001</v>
       </c>
       <c r="D131">
         <v>4.369333333333334</v>
@@ -3454,7 +3454,7 @@
         <v>3.843541666666667</v>
       </c>
       <c r="E133">
-        <v>-3.602708333333333</v>
+        <v>-3.602708333333334</v>
       </c>
       <c r="F133">
         <v>89.83333333333333</v>
@@ -3468,7 +3468,7 @@
         <v>44193</v>
       </c>
       <c r="B134">
-        <v>8.385000000000003</v>
+        <v>8.385</v>
       </c>
       <c r="C134">
         <v>8.796250000000001</v>
@@ -3520,7 +3520,7 @@
         <v>6.860458333333334</v>
       </c>
       <c r="D136">
-        <v>3.011208333333333</v>
+        <v>3.011208333333334</v>
       </c>
       <c r="E136">
         <v>-1.097375</v>
@@ -3537,16 +3537,16 @@
         <v>44196</v>
       </c>
       <c r="B137">
-        <v>4.491999999999998</v>
+        <v>4.492</v>
       </c>
       <c r="C137">
-        <v>6.221250000000002</v>
+        <v>6.22125</v>
       </c>
       <c r="D137">
         <v>2.43925</v>
       </c>
       <c r="E137">
-        <v>0.6207083333333334</v>
+        <v>0.6207083333333333</v>
       </c>
       <c r="F137">
         <v>94.16666666666667</v>
@@ -3563,7 +3563,7 @@
         <v>4.398625</v>
       </c>
       <c r="C138">
-        <v>6.160875000000001</v>
+        <v>6.160875</v>
       </c>
       <c r="D138">
         <v>2.647416666666667</v>
@@ -3583,10 +3583,10 @@
         <v>44198</v>
       </c>
       <c r="B139">
-        <v>4.666916666666668</v>
+        <v>4.666916666666666</v>
       </c>
       <c r="C139">
-        <v>6.278416666666668</v>
+        <v>6.278416666666666</v>
       </c>
       <c r="D139">
         <v>2.853541666666667</v>
@@ -3606,7 +3606,7 @@
         <v>44199</v>
       </c>
       <c r="B140">
-        <v>4.956541666666667</v>
+        <v>4.956541666666666</v>
       </c>
       <c r="C140">
         <v>6.35425</v>
@@ -3629,13 +3629,13 @@
         <v>44200</v>
       </c>
       <c r="B141">
-        <v>5.212916666666668</v>
+        <v>5.212916666666667</v>
       </c>
       <c r="C141">
-        <v>6.297416666666666</v>
+        <v>6.297416666666667</v>
       </c>
       <c r="D141">
-        <v>3.153250000000001</v>
+        <v>3.15325</v>
       </c>
       <c r="E141">
         <v>-5.379083333333334</v>
@@ -3655,7 +3655,7 @@
         <v>5.573708333333333</v>
       </c>
       <c r="C142">
-        <v>5.995333333333332</v>
+        <v>5.995333333333334</v>
       </c>
       <c r="D142">
         <v>3.358416666666667</v>
@@ -3675,7 +3675,7 @@
         <v>44202</v>
       </c>
       <c r="B143">
-        <v>5.999499999999999</v>
+        <v>5.9995</v>
       </c>
       <c r="C143">
         <v>6.131208333333333</v>
@@ -3698,16 +3698,16 @@
         <v>44203</v>
       </c>
       <c r="B144">
-        <v>6.257666666666668</v>
+        <v>6.257666666666666</v>
       </c>
       <c r="C144">
-        <v>6.099333333333331</v>
+        <v>6.099333333333333</v>
       </c>
       <c r="D144">
         <v>3.640416666666667</v>
       </c>
       <c r="E144">
-        <v>-6.892750000000002</v>
+        <v>-6.892749999999999</v>
       </c>
       <c r="F144">
         <v>90.375</v>
@@ -3721,7 +3721,7 @@
         <v>44204</v>
       </c>
       <c r="B145">
-        <v>6.457166666666666</v>
+        <v>6.457166666666667</v>
       </c>
       <c r="C145">
         <v>6.082166666666667</v>
@@ -3750,7 +3750,7 @@
         <v>6.130583333333334</v>
       </c>
       <c r="D146">
-        <v>4.085041666666665</v>
+        <v>4.085041666666666</v>
       </c>
       <c r="E146">
         <v>-15.97583333333333</v>
@@ -3770,7 +3770,7 @@
         <v>6.584083333333333</v>
       </c>
       <c r="C147">
-        <v>6.122208333333334</v>
+        <v>6.122208333333333</v>
       </c>
       <c r="D147">
         <v>4.255666666666666</v>
@@ -3793,13 +3793,13 @@
         <v>6.461541666666666</v>
       </c>
       <c r="C148">
-        <v>6.152166666666669</v>
+        <v>6.152166666666666</v>
       </c>
       <c r="D148">
         <v>3.929333333333334</v>
       </c>
       <c r="E148">
-        <v>-9.769166666666669</v>
+        <v>-9.769166666666667</v>
       </c>
       <c r="F148">
         <v>86.75</v>
@@ -3813,13 +3813,13 @@
         <v>44208</v>
       </c>
       <c r="B149">
-        <v>4.838833333333333</v>
+        <v>4.838833333333334</v>
       </c>
       <c r="C149">
         <v>5.298666666666667</v>
       </c>
       <c r="D149">
-        <v>3.815041666666666</v>
+        <v>3.815041666666667</v>
       </c>
       <c r="E149">
         <v>-11.78166666666667</v>
@@ -3839,7 +3839,7 @@
         <v>2.662166666666667</v>
       </c>
       <c r="C150">
-        <v>3.029541666666668</v>
+        <v>3.029541666666667</v>
       </c>
       <c r="D150">
         <v>2.538458333333333</v>
@@ -3865,7 +3865,7 @@
         <v>2.725625</v>
       </c>
       <c r="D151">
-        <v>1.576458333333334</v>
+        <v>1.576458333333333</v>
       </c>
       <c r="E151">
         <v>-23.07625</v>
@@ -3882,13 +3882,13 @@
         <v>44211</v>
       </c>
       <c r="B152">
-        <v>3.459208333333334</v>
+        <v>3.459208333333333</v>
       </c>
       <c r="C152">
-        <v>3.266458333333334</v>
+        <v>3.266458333333333</v>
       </c>
       <c r="D152">
-        <v>0.9529166666666669</v>
+        <v>0.9529166666666667</v>
       </c>
       <c r="E152">
         <v>-20.69625</v>
@@ -3905,13 +3905,13 @@
         <v>44212</v>
       </c>
       <c r="B153">
-        <v>4.158708333333334</v>
+        <v>4.158708333333333</v>
       </c>
       <c r="C153">
-        <v>3.633166666666667</v>
+        <v>3.633166666666666</v>
       </c>
       <c r="D153">
-        <v>0.7824166666666668</v>
+        <v>0.7824166666666666</v>
       </c>
       <c r="E153">
         <v>-17.11958333333333</v>
@@ -3928,7 +3928,7 @@
         <v>44213</v>
       </c>
       <c r="B154">
-        <v>4.623875000000001</v>
+        <v>4.623875</v>
       </c>
       <c r="C154">
         <v>4.003416666666666</v>
@@ -3951,13 +3951,13 @@
         <v>44214</v>
       </c>
       <c r="B155">
-        <v>4.726250000000001</v>
+        <v>4.72625</v>
       </c>
       <c r="C155">
-        <v>4.109166666666666</v>
+        <v>4.109166666666667</v>
       </c>
       <c r="D155">
-        <v>0.8497083333333332</v>
+        <v>0.8497083333333334</v>
       </c>
       <c r="E155">
         <v>-5.680083333333333</v>
@@ -3983,7 +3983,7 @@
         <v>1.142708333333333</v>
       </c>
       <c r="E156">
-        <v>-3.523083333333333</v>
+        <v>-3.523083333333334</v>
       </c>
       <c r="F156">
         <v>93.79166666666667</v>
@@ -3997,7 +3997,7 @@
         <v>44216</v>
       </c>
       <c r="B157">
-        <v>4.459958333333333</v>
+        <v>4.459958333333334</v>
       </c>
       <c r="C157">
         <v>4.118916666666666</v>
@@ -4006,7 +4006,7 @@
         <v>1.427958333333333</v>
       </c>
       <c r="E157">
-        <v>-4.509416666666666</v>
+        <v>-4.509416666666667</v>
       </c>
       <c r="F157">
         <v>91.70833333333333</v>
@@ -4072,10 +4072,10 @@
         <v>1.257458333333333</v>
       </c>
       <c r="D160">
-        <v>-0.07645833333333331</v>
+        <v>-0.07645833333333334</v>
       </c>
       <c r="E160">
-        <v>-2.986749999999999</v>
+        <v>-2.98675</v>
       </c>
       <c r="F160">
         <v>93.33333333333333</v>
@@ -4098,7 +4098,7 @@
         <v>0.1312916666666667</v>
       </c>
       <c r="E161">
-        <v>0.5332499999999999</v>
+        <v>0.53325</v>
       </c>
       <c r="F161">
         <v>96.33333333333333</v>
@@ -4118,10 +4118,10 @@
         <v>1.240791666666667</v>
       </c>
       <c r="D162">
-        <v>-0.05679166666666668</v>
+        <v>-0.05679166666666666</v>
       </c>
       <c r="E162">
-        <v>0.3883749999999999</v>
+        <v>0.388375</v>
       </c>
       <c r="F162">
         <v>97.625</v>
@@ -4144,7 +4144,7 @@
         <v>0.220375</v>
       </c>
       <c r="E163">
-        <v>0.4143749999999999</v>
+        <v>0.414375</v>
       </c>
       <c r="F163">
         <v>94.70833333333333</v>
@@ -4167,7 +4167,7 @@
         <v>0.3619583333333333</v>
       </c>
       <c r="E164">
-        <v>0.2362916666666668</v>
+        <v>0.2362916666666667</v>
       </c>
       <c r="F164">
         <v>98.25</v>
@@ -4187,7 +4187,7 @@
         <v>1.183708333333333</v>
       </c>
       <c r="D165">
-        <v>0.4088333333333334</v>
+        <v>0.4088333333333333</v>
       </c>
       <c r="E165">
         <v>-1.4785</v>
@@ -4210,7 +4210,7 @@
         <v>1.08875</v>
       </c>
       <c r="D166">
-        <v>0.4860416666666669</v>
+        <v>0.4860416666666666</v>
       </c>
       <c r="E166">
         <v>-2.829083333333333</v>
@@ -4227,10 +4227,10 @@
         <v>44226</v>
       </c>
       <c r="B167">
-        <v>-2.000583333333334</v>
+        <v>-2.000583333333333</v>
       </c>
       <c r="C167">
-        <v>0.8100833333333332</v>
+        <v>0.8100833333333334</v>
       </c>
       <c r="D167">
         <v>0.6259166666666667</v>
@@ -4253,10 +4253,10 @@
         <v>-1.535416666666667</v>
       </c>
       <c r="C168">
-        <v>0.9982916666666668</v>
+        <v>0.9982916666666667</v>
       </c>
       <c r="D168">
-        <v>0.4833333333333334</v>
+        <v>0.4833333333333333</v>
       </c>
       <c r="E168">
         <v>-5.493041666666667</v>
@@ -4276,7 +4276,7 @@
         <v>-1.266958333333333</v>
       </c>
       <c r="C169">
-        <v>0.9773749999999999</v>
+        <v>0.977375</v>
       </c>
       <c r="D169">
         <v>0.355125</v>
@@ -4296,7 +4296,7 @@
         <v>44229</v>
       </c>
       <c r="B170">
-        <v>-0.8047083333333331</v>
+        <v>-0.8047083333333332</v>
       </c>
       <c r="C170">
         <v>0.8126666666666668</v>
@@ -4305,7 +4305,7 @@
         <v>0.1358333333333333</v>
       </c>
       <c r="E170">
-        <v>-17.80416666666666</v>
+        <v>-17.80416666666667</v>
       </c>
       <c r="F170">
         <v>83.45833333333333</v>
@@ -4388,7 +4388,7 @@
         <v>44233</v>
       </c>
       <c r="B174">
-        <v>2.692708333333334</v>
+        <v>2.692708333333333</v>
       </c>
       <c r="C174">
         <v>1.5005</v>
@@ -4414,10 +4414,10 @@
         <v>3.258916666666666</v>
       </c>
       <c r="C175">
-        <v>1.733791666666666</v>
+        <v>1.733791666666667</v>
       </c>
       <c r="D175">
-        <v>0.9027083333333331</v>
+        <v>0.9027083333333333</v>
       </c>
       <c r="E175">
         <v>-8.535291666666668</v>
@@ -4437,10 +4437,10 @@
         <v>3.650166666666667</v>
       </c>
       <c r="C176">
-        <v>1.910791666666666</v>
+        <v>1.910791666666667</v>
       </c>
       <c r="D176">
-        <v>1.207458333333334</v>
+        <v>1.207458333333333</v>
       </c>
       <c r="E176">
         <v>-10.31416666666667</v>
@@ -4460,7 +4460,7 @@
         <v>3.806</v>
       </c>
       <c r="C177">
-        <v>2.031200000000001</v>
+        <v>2.0312</v>
       </c>
       <c r="D177">
         <v>1.4308</v>

</xml_diff>